<commit_message>
Add RWP access type.
</commit_message>
<xml_diff>
--- a/excels/block1.xlsx
+++ b/excels/block1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhang\git\RegisterPrinter\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAA414A-0FE1-487B-9121-568F811D5CF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032C50F0-CC8D-4B1E-86C3-146E0D1ABE1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{C83E0548-C80E-4E67-B2D8-AA055AFEE83E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C83E0548-C80E-4E67-B2D8-AA055AFEE83E}"/>
   </bookViews>
   <sheets>
     <sheet name="Type1" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -106,11 +100,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>RW</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Register1-Field1 注释</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RWP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -478,7 +472,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -520,13 +514,13 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" t="s">
         <v>18</v>
-      </c>
-      <c r="G5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -540,7 +534,7 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
         <v>7</v>

</xml_diff>